<commit_message>
remove .dat files from previous runs; update tiny protein example
</commit_message>
<xml_diff>
--- a/test/4LAJ.cmrf/results/discrete-vs-continuous-pf.xlsx
+++ b/test/4LAJ.cmrf/results/discrete-vs-continuous-pf.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MCIC/Documents/GitHub/adi/OSPREY_refactor/test/4LAJ.cmrf/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MCIC/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33320" yWindow="5560" windowWidth="17840" windowHeight="16380" tabRatio="500"/>
+    <workbookView xWindow="26500" yWindow="460" windowWidth="17500" windowHeight="13080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="4LAJ" sheetId="1" r:id="rId1"/>
@@ -27,16 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
-  <si>
-    <t>Mutabke Residues</t>
-  </si>
-  <si>
-    <t>ARG-419</t>
-  </si>
-  <si>
-    <t>THR-702</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="10">
   <si>
     <t>SCMF</t>
   </si>
@@ -53,13 +44,19 @@
     <t>K* (pairwise lb)</t>
   </si>
   <si>
-    <t>MET-711</t>
-  </si>
-  <si>
-    <t>LYS-421</t>
-  </si>
-  <si>
-    <t>ARG-645</t>
+    <t>Mutable Residues</t>
+  </si>
+  <si>
+    <t>ARG-419 THR-702</t>
+  </si>
+  <si>
+    <t>ARG-419 MET-711</t>
+  </si>
+  <si>
+    <t>LYS-421 ARG-645</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
   </si>
 </sst>
 </file>
@@ -375,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -386,130 +383,150 @@
     <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>3</v>
       </c>
       <c r="B6" s="1">
         <v>8.4277520812247602</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E6" s="1">
         <v>8.9124894970067601</v>
       </c>
       <c r="G6" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1">
-        <v>10.104975621275701</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>28.38</v>
+      </c>
+      <c r="J6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1">
         <v>47.260773290946403</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E7" s="1">
         <v>52.969230119857599</v>
       </c>
       <c r="G7" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H7" s="1">
-        <v>66.247521054922998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>84.4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1">
         <v>29.65</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E8" s="1">
         <v>38.89</v>
       </c>
       <c r="G8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H8" s="1">
         <v>50.317917450700001</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1">
         <v>30.28</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E9" s="1">
         <v>38.93</v>
       </c>
       <c r="G9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H9" s="1">
         <v>50.394810025699996</v>
+      </c>
+      <c r="J9" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>